<commit_message>
Added nice summary display to tournament script
slight modification to jp3 for comparison
</commit_message>
<xml_diff>
--- a/OpponentAnalysis.xlsx
+++ b/OpponentAnalysis.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB1E7D3-5906-401F-A645-2EEB92DFAD32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73B78DC-594B-471C-AE43-9AFB1297587C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>Mallin Moolman</t>
   </si>
@@ -118,13 +118,73 @@
     <t>Matthew Holmes</t>
   </si>
   <si>
-    <t>only beat me by 20-odd points!  Went to score</t>
-  </si>
-  <si>
     <t>kiting at the end, made a cockup and he shot me</t>
   </si>
   <si>
     <t>broken</t>
+  </si>
+  <si>
+    <t>lost</t>
+  </si>
+  <si>
+    <t>won</t>
+  </si>
+  <si>
+    <t>aka "kuifie".  Looks like he goes for the health and then attacks the nearest work.  No digging except to get to opponents</t>
+  </si>
+  <si>
+    <t>only beat me by 20-odd points!  Went to score.  Not aggressive, looks like his digging is more optimal than mine</t>
+  </si>
+  <si>
+    <t>aggressive, looks like he fumbles around a bit when trying to get a shot.  Really shouldn't have lost to this bot!</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>bot name</t>
+  </si>
+  <si>
+    <t>kuifie</t>
+  </si>
+  <si>
+    <t>jiro</t>
+  </si>
+  <si>
+    <t>BurgerB</t>
+  </si>
+  <si>
+    <t>looks like hes doing some kind of tree search because he digs pretty nicely and shoots oppurtunistically.  His last work got stuck moving between 2 spaces</t>
+  </si>
+  <si>
+    <t># "lost" worms</t>
+  </si>
+  <si>
+    <t>got stuck in a loop at the end, somehow he got a final shot in?</t>
+  </si>
+  <si>
+    <t>weird last shot "bug"</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>looks like he runs for health and then starts digging.  I seem to have gotten lucky with skirmishes but he won on points.</t>
+  </si>
+  <si>
+    <t>I placed here…</t>
+  </si>
+  <si>
+    <t>SandWorm</t>
+  </si>
+  <si>
+    <t>nope</t>
+  </si>
+  <si>
+    <t>beat me by 130.  Looks like he's doing some kind of tree search, but better than me…His bots all ended up in the middle, not sure if that was coincidental</t>
   </si>
 </sst>
 </file>
@@ -442,202 +502,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="F22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
-        <v>34</v>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug where loss wasn't being penalised
changed name of method
</commit_message>
<xml_diff>
--- a/OpponentAnalysis.xlsx
+++ b/OpponentAnalysis.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73B78DC-594B-471C-AE43-9AFB1297587C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A26F6B-F49A-4B50-BE5A-7FFC9C9D7417}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
   <si>
     <t>Mallin Moolman</t>
   </si>
@@ -185,6 +185,30 @@
   </si>
   <si>
     <t>beat me by 130.  Looks like he's doing some kind of tree search, but better than me…His bots all ended up in the middle, not sure if that was coincidental</t>
+  </si>
+  <si>
+    <t>Digitum Dei</t>
+  </si>
+  <si>
+    <t>rushed for the middle and then seemed to get confused.  Maybe a poor implementation of a search tree?</t>
+  </si>
+  <si>
+    <t>one worm rushed for health packs, and then digging commenced</t>
+  </si>
+  <si>
+    <t>Ikabot</t>
+  </si>
+  <si>
+    <t>Steam powered worm</t>
+  </si>
+  <si>
+    <t>lost by KO.  He was doing some fancy dodging in the skirmishes! But I still won the first one tho</t>
+  </si>
+  <si>
+    <t>Marvijo</t>
+  </si>
+  <si>
+    <t>rushed for the middle and then just hung around there?  I went on digging merrily and won by points</t>
   </si>
 </sst>
 </file>
@@ -504,19 +528,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -533,7 +557,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -544,7 +568,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -552,7 +576,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -572,12 +596,21 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -591,7 +624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -602,12 +635,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -615,27 +657,27 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -646,22 +688,31 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -675,22 +726,22 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -707,22 +758,31 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -736,12 +796,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -752,7 +812,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -763,7 +823,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -774,7 +834,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -785,7 +845,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -796,7 +856,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -807,7 +867,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>

</xml_diff>